<commit_message>
product master xlsx file updated. product hierarchy button added
</commit_message>
<xml_diff>
--- a/adminDashboard/files/productMaster_sample.xlsx
+++ b/adminDashboard/files/productMaster_sample.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t xml:space="preserve">Sr.No</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Itemcode</t>
   </si>
@@ -46,58 +43,58 @@
     <t xml:space="preserve">ParentItemName</t>
   </si>
   <si>
+    <t xml:space="preserve">Isactive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LengthUoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WidthUoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeightUoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VolumeUoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WeightUoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supersessionitem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ManageSerialNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsConsumable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsRecommended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsSlowmoving</t>
+  </si>
+  <si>
     <t xml:space="preserve">Itemgroup</t>
   </si>
   <si>
     <t xml:space="preserve">GroupDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isactive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LengthUoM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Width</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WidthUoM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeightUoM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VolumeUoM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WeightUoM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supersessionitem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ManageSerialNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IsConsumable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IsRecommended</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IsSlowmoving</t>
   </si>
   <si>
     <t xml:space="preserve">ImageName</t>
@@ -118,6 +115,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,6 +137,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -155,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -170,6 +169,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -196,13 +202,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -282,102 +296,163 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I4" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
product master data updated. order confirm added quotatn.
</commit_message>
<xml_diff>
--- a/adminDashboard/files/productMaster_sample.xlsx
+++ b/adminDashboard/files/productMaster_sample.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+  <si>
+    <t xml:space="preserve">Model # </t>
+  </si>
   <si>
     <t xml:space="preserve">Itemcode</t>
   </si>
@@ -31,13 +34,13 @@
     <t xml:space="preserve">ShortCode</t>
   </si>
   <si>
-    <t xml:space="preserve">Itemtype</t>
+    <t xml:space="preserve">Itemtype (Machine/SpareParts/Merchandise)</t>
   </si>
   <si>
     <t xml:space="preserve">FamilyCode</t>
   </si>
   <si>
-    <t xml:space="preserve">FamilyDesc</t>
+    <t xml:space="preserve">FamilyDesc (Commercial / LM Home / Grinder / Modbar / Water Filter / GS3)</t>
   </si>
   <si>
     <t xml:space="preserve">ParentItemName</t>
@@ -94,21 +97,116 @@
     <t xml:space="preserve">Itemgroup</t>
   </si>
   <si>
-    <t xml:space="preserve">GroupDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ImageName</t>
+    <t xml:space="preserve">GroupDescription </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image Name </t>
   </si>
   <si>
     <t xml:space="preserve">PartRefNum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boiler Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PID Temperature Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pump Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicator Lights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steam Boiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Reservoir capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2GPBAVSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCREW M10X25 SOCKET CAP S/S A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I.1.073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpareParts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">linea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commercial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 - BODY PANEL ASSEMBLY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPMAVI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">screws, nuts, bolts, washers…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 - BODY PANEL ASSEMBLY.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIGH LEG LINEA PB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.3.007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPMACR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panels and external parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -133,14 +231,14 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,23 +248,28 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -198,25 +301,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -231,7 +356,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -248,7 +373,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -279,7 +404,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00B050"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -296,163 +421,325 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A2:AK4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.8418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.515306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="80.2142857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.719387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.48469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.68367346938776"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.51530612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.1020408163265"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.20408163265306"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.7959183673469"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.93877551020408"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.515306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.3316326530612"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="24.219387755102"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.9336734693878"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.0204081632653"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="26.4387755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="29.9132653061224"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.7959183673469"/>
+    <col collapsed="false" hidden="false" max="35" min="29" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="6.98469387755102"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="5.31632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
+    <row r="2" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
+      <c r="A3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="8" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I4" s="3"/>
+      <c r="A4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5" t="n">
+        <v>1897.3</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="8" t="n">
+        <v>197.83</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>